<commit_message>
Cap nhat phan trang
</commit_message>
<xml_diff>
--- a/admin/upload_excel/uploads/sanpham.xlsx
+++ b/admin/upload_excel/uploads/sanpham.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dulieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4429C569-8420-4DD8-B7C2-6C8547D7AB19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7995" xr2:uid="{B9A2076C-84CF-4F1F-BC4C-D617F90B8E76}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -996,7 +995,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1425,12 +1424,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB59ADC8-2F5B-4006-9DA9-FA86B053B636}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,10 +1596,10 @@
         <v>10</v>
       </c>
       <c r="I2" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J2" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>157</v>
@@ -1682,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="I3" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J3" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>157</v>
@@ -1767,10 +1766,10 @@
         <v>10</v>
       </c>
       <c r="I4" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J4" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>157</v>
@@ -1852,10 +1851,10 @@
         <v>10</v>
       </c>
       <c r="I5" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>157</v>
@@ -1937,10 +1936,10 @@
         <v>10</v>
       </c>
       <c r="I6" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J6" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>157</v>
@@ -2022,10 +2021,10 @@
         <v>10</v>
       </c>
       <c r="I7" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>158</v>
@@ -2109,10 +2108,10 @@
         <v>10</v>
       </c>
       <c r="I8" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>158</v>
@@ -2196,10 +2195,10 @@
         <v>10</v>
       </c>
       <c r="I9" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>158</v>
@@ -2283,10 +2282,10 @@
         <v>10</v>
       </c>
       <c r="I10" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>158</v>
@@ -2370,10 +2369,10 @@
         <v>10</v>
       </c>
       <c r="I11" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>236</v>
@@ -2457,10 +2456,10 @@
         <v>10</v>
       </c>
       <c r="I12" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>236</v>
@@ -2544,10 +2543,10 @@
         <v>10</v>
       </c>
       <c r="I13" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>236</v>
@@ -2631,10 +2630,10 @@
         <v>10</v>
       </c>
       <c r="I14" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>236</v>
@@ -2718,10 +2717,10 @@
         <v>10</v>
       </c>
       <c r="I15" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J15" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>159</v>
@@ -2803,10 +2802,10 @@
         <v>10</v>
       </c>
       <c r="I16" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J16" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>159</v>
@@ -2888,10 +2887,10 @@
         <v>10</v>
       </c>
       <c r="I17" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J17" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>159</v>
@@ -2973,10 +2972,10 @@
         <v>10</v>
       </c>
       <c r="I18" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J18" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>159</v>
@@ -3058,10 +3057,10 @@
         <v>10</v>
       </c>
       <c r="I19" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>157</v>
@@ -3143,10 +3142,10 @@
         <v>10</v>
       </c>
       <c r="I20" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J20" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>157</v>
@@ -3228,10 +3227,10 @@
         <v>10</v>
       </c>
       <c r="I21" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J21" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>157</v>
@@ -3313,10 +3312,10 @@
         <v>10</v>
       </c>
       <c r="I22" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J22" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>157</v>
@@ -3398,10 +3397,10 @@
         <v>10</v>
       </c>
       <c r="I23" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23" s="10">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>158</v>
@@ -3485,10 +3484,10 @@
         <v>10</v>
       </c>
       <c r="I24" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24" s="10">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>158</v>
@@ -3572,10 +3571,10 @@
         <v>10</v>
       </c>
       <c r="I25" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25" s="10">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>158</v>
@@ -3659,10 +3658,10 @@
         <v>10</v>
       </c>
       <c r="I26" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26" s="10">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>158</v>
@@ -3746,10 +3745,10 @@
         <v>10</v>
       </c>
       <c r="I27" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>236</v>
@@ -3833,10 +3832,10 @@
         <v>10</v>
       </c>
       <c r="I28" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>236</v>
@@ -3920,10 +3919,10 @@
         <v>10</v>
       </c>
       <c r="I29" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>236</v>
@@ -4007,10 +4006,10 @@
         <v>10</v>
       </c>
       <c r="I30" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>236</v>
@@ -4094,10 +4093,10 @@
         <v>10</v>
       </c>
       <c r="I31" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J31" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>159</v>
@@ -4179,10 +4178,10 @@
         <v>10</v>
       </c>
       <c r="I32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J32" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>159</v>
@@ -4264,10 +4263,10 @@
         <v>10</v>
       </c>
       <c r="I33" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J33" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>159</v>
@@ -4349,10 +4348,10 @@
         <v>10</v>
       </c>
       <c r="I34" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J34" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>159</v>
@@ -4434,10 +4433,10 @@
         <v>10</v>
       </c>
       <c r="I35" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J35" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>159</v>
@@ -4519,10 +4518,10 @@
         <v>10</v>
       </c>
       <c r="I36" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J36" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>157</v>
@@ -4604,10 +4603,10 @@
         <v>10</v>
       </c>
       <c r="I37" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>157</v>
@@ -4689,10 +4688,10 @@
         <v>10</v>
       </c>
       <c r="I38" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J38" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>157</v>
@@ -4774,10 +4773,10 @@
         <v>10</v>
       </c>
       <c r="I39" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J39" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>157</v>
@@ -4859,10 +4858,10 @@
         <v>10</v>
       </c>
       <c r="I40" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J40" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>157</v>
@@ -4944,10 +4943,10 @@
         <v>10</v>
       </c>
       <c r="I41" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>158</v>
@@ -5031,10 +5030,10 @@
         <v>10</v>
       </c>
       <c r="I42" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>158</v>
@@ -5118,10 +5117,10 @@
         <v>10</v>
       </c>
       <c r="I43" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J43" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>158</v>
@@ -5205,10 +5204,10 @@
         <v>10</v>
       </c>
       <c r="I44" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>158</v>
@@ -5292,10 +5291,10 @@
         <v>10</v>
       </c>
       <c r="I45" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J45" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>158</v>
@@ -5377,10 +5376,10 @@
         <v>10</v>
       </c>
       <c r="I46" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J46" s="10">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>236</v>
@@ -5462,10 +5461,10 @@
         <v>10</v>
       </c>
       <c r="I47" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J47" s="10">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>159</v>
@@ -5545,10 +5544,10 @@
         <v>10</v>
       </c>
       <c r="I48" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J48" s="10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>157</v>
@@ -5628,10 +5627,10 @@
         <v>10</v>
       </c>
       <c r="I49" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J49" s="10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>158</v>
@@ -5713,10 +5712,10 @@
         <v>10</v>
       </c>
       <c r="I50" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J50" s="10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>236</v>
@@ -5798,10 +5797,10 @@
         <v>10</v>
       </c>
       <c r="I51" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J51" s="10">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>159</v>
@@ -5881,10 +5880,10 @@
         <v>10</v>
       </c>
       <c r="I52" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>157</v>
@@ -5964,10 +5963,10 @@
         <v>10</v>
       </c>
       <c r="I53" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J53" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>158</v>
@@ -6049,10 +6048,10 @@
         <v>10</v>
       </c>
       <c r="I54" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J54" s="10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>236</v>
@@ -6134,10 +6133,10 @@
         <v>10</v>
       </c>
       <c r="I55" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J55" s="10">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>159</v>
@@ -6217,10 +6216,10 @@
         <v>10</v>
       </c>
       <c r="I56" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J56" s="10">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>157</v>
@@ -6300,10 +6299,10 @@
         <v>10</v>
       </c>
       <c r="I57" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" s="10">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>158</v>
@@ -6385,10 +6384,10 @@
         <v>10</v>
       </c>
       <c r="I58" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J58" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>236</v>
@@ -6470,10 +6469,10 @@
         <v>10</v>
       </c>
       <c r="I59" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J59" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>159</v>
@@ -6553,10 +6552,10 @@
         <v>10</v>
       </c>
       <c r="I60" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J60" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>157</v>
@@ -6636,10 +6635,10 @@
         <v>10</v>
       </c>
       <c r="I61" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J61" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>158</v>
@@ -6721,10 +6720,10 @@
         <v>10</v>
       </c>
       <c r="I62" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" s="10">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>236</v>
@@ -6808,10 +6807,10 @@
         <v>10</v>
       </c>
       <c r="I63" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J63" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>159</v>
@@ -6893,10 +6892,10 @@
         <v>10</v>
       </c>
       <c r="I64" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J64" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>157</v>
@@ -6978,10 +6977,10 @@
         <v>10</v>
       </c>
       <c r="I65" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J65" s="10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>158</v>
@@ -7065,10 +7064,10 @@
         <v>10</v>
       </c>
       <c r="I66" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J66" s="10">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>159</v>
@@ -7150,10 +7149,10 @@
         <v>10</v>
       </c>
       <c r="I67" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J67" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>157</v>
@@ -7235,10 +7234,10 @@
         <v>10</v>
       </c>
       <c r="I68" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J68" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>158</v>
@@ -7322,10 +7321,10 @@
         <v>10</v>
       </c>
       <c r="I69" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J69" s="10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>236</v>
@@ -7409,10 +7408,10 @@
         <v>10</v>
       </c>
       <c r="I70" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J70" s="10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>159</v>
@@ -7494,10 +7493,10 @@
         <v>10</v>
       </c>
       <c r="I71" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J71" s="10">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>157</v>
@@ -7579,10 +7578,10 @@
         <v>10</v>
       </c>
       <c r="I72" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J72" s="10">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>158</v>
@@ -7666,10 +7665,10 @@
         <v>10</v>
       </c>
       <c r="I73" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J73" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>236</v>
@@ -7753,10 +7752,10 @@
         <v>10</v>
       </c>
       <c r="I74" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74" s="10">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>159</v>
@@ -7838,10 +7837,10 @@
         <v>10</v>
       </c>
       <c r="I75" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J75" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>157</v>
@@ -7923,10 +7922,10 @@
         <v>10</v>
       </c>
       <c r="I76" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J76" s="10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>158</v>
@@ -8010,10 +8009,10 @@
         <v>10</v>
       </c>
       <c r="I77" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J77" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>236</v>
@@ -8097,10 +8096,10 @@
         <v>10</v>
       </c>
       <c r="I78" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J78" s="10">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>159</v>
@@ -8182,10 +8181,10 @@
         <v>10</v>
       </c>
       <c r="I79" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J79" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>157</v>
@@ -8267,10 +8266,10 @@
         <v>10</v>
       </c>
       <c r="I80" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J80" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>159</v>
@@ -8352,10 +8351,10 @@
         <v>10</v>
       </c>
       <c r="I81" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J81" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>171</v>
@@ -8439,10 +8438,10 @@
         <v>10</v>
       </c>
       <c r="I82" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J82" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>158</v>
@@ -8526,10 +8525,10 @@
         <v>10</v>
       </c>
       <c r="I83" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J83" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>171</v>
@@ -8613,10 +8612,10 @@
         <v>10</v>
       </c>
       <c r="I84" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J84" s="10">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>158</v>
@@ -8700,10 +8699,10 @@
         <v>10</v>
       </c>
       <c r="I85" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J85" s="10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>158</v>
@@ -8787,10 +8786,10 @@
         <v>10</v>
       </c>
       <c r="I86" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J86" s="10">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>157</v>
@@ -8872,10 +8871,10 @@
         <v>10</v>
       </c>
       <c r="I87" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J87" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>171</v>
@@ -8959,10 +8958,10 @@
         <v>10</v>
       </c>
       <c r="I88" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J88" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>158</v>
@@ -9046,10 +9045,10 @@
         <v>10</v>
       </c>
       <c r="I89" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J89" s="10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Cap nhat don hang
</commit_message>
<xml_diff>
--- a/admin/upload_excel/uploads/sanpham.xlsx
+++ b/admin/upload_excel/uploads/sanpham.xlsx
@@ -1554,9 +1554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,9 +3532,7 @@
       <c r="K23" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L23" s="8">
-        <v>-3</v>
-      </c>
+      <c r="L23" s="8"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
       <c r="O23" s="10">
@@ -3619,9 +3617,7 @@
       <c r="K24" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L24" s="8">
-        <v>-2</v>
-      </c>
+      <c r="L24" s="8"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="10">
@@ -3706,9 +3702,7 @@
       <c r="K25" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L25" s="8">
-        <v>-1</v>
-      </c>
+      <c r="L25" s="8"/>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="10">
@@ -3793,9 +3787,7 @@
       <c r="K26" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L26" s="8">
-        <v>0</v>
-      </c>
+      <c r="L26" s="8"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
       <c r="O26" s="10">
@@ -5078,9 +5070,7 @@
       <c r="K41" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L41" s="8">
-        <v>-4</v>
-      </c>
+      <c r="L41" s="8"/>
       <c r="M41" s="11"/>
       <c r="N41" s="11"/>
       <c r="O41" s="10">
@@ -5165,9 +5155,7 @@
       <c r="K42" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L42" s="8">
-        <v>-3</v>
-      </c>
+      <c r="L42" s="8"/>
       <c r="M42" s="11"/>
       <c r="N42" s="11"/>
       <c r="O42" s="10">
@@ -5252,9 +5240,7 @@
       <c r="K43" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L43" s="8">
-        <v>-2</v>
-      </c>
+      <c r="L43" s="8"/>
       <c r="M43" s="11"/>
       <c r="N43" s="11"/>
       <c r="O43" s="10">
@@ -5339,9 +5325,7 @@
       <c r="K44" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L44" s="8">
-        <v>-1</v>
-      </c>
+      <c r="L44" s="8"/>
       <c r="M44" s="11"/>
       <c r="N44" s="11"/>
       <c r="O44" s="10">
@@ -5426,9 +5410,7 @@
       <c r="K45" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L45" s="8">
-        <v>0</v>
-      </c>
+      <c r="L45" s="8"/>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
       <c r="O45" s="10">
@@ -5762,9 +5744,7 @@
       <c r="K49" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L49" s="8">
-        <v>0</v>
-      </c>
+      <c r="L49" s="8"/>
       <c r="M49" s="11"/>
       <c r="N49" s="11"/>
       <c r="O49" s="10">
@@ -6098,9 +6078,7 @@
       <c r="K53" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L53" s="8">
-        <v>0</v>
-      </c>
+      <c r="L53" s="8"/>
       <c r="M53" s="11"/>
       <c r="N53" s="11"/>
       <c r="O53" s="10">
@@ -6434,9 +6412,7 @@
       <c r="K57" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L57" s="8">
-        <v>0</v>
-      </c>
+      <c r="L57" s="8"/>
       <c r="M57" s="11"/>
       <c r="N57" s="11"/>
       <c r="O57" s="10">
@@ -6770,9 +6746,7 @@
       <c r="K61" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L61" s="8">
-        <v>0</v>
-      </c>
+      <c r="L61" s="8"/>
       <c r="M61" s="11"/>
       <c r="N61" s="11"/>
       <c r="O61" s="10">
@@ -7197,9 +7171,7 @@
       <c r="K66" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L66" s="8">
-        <v>0</v>
-      </c>
+      <c r="L66" s="8"/>
       <c r="M66" s="11"/>
       <c r="N66" s="11"/>
       <c r="O66" s="10">
@@ -7541,9 +7513,7 @@
       <c r="K70" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L70" s="8">
-        <v>0</v>
-      </c>
+      <c r="L70" s="8"/>
       <c r="M70" s="11"/>
       <c r="N70" s="11"/>
       <c r="O70" s="10">
@@ -7877,9 +7847,7 @@
       <c r="K74" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L74" s="8">
-        <v>0</v>
-      </c>
+      <c r="L74" s="8"/>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
       <c r="O74" s="10">
@@ -8304,9 +8272,7 @@
       <c r="K79" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L79" s="8">
-        <v>0</v>
-      </c>
+      <c r="L79" s="8"/>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
       <c r="O79" s="10">
@@ -8561,9 +8527,7 @@
       <c r="K82" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L82" s="8">
-        <v>0</v>
-      </c>
+      <c r="L82" s="8"/>
       <c r="M82" s="11"/>
       <c r="N82" s="11"/>
       <c r="O82" s="10">
@@ -8905,9 +8869,7 @@
       <c r="K86" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L86" s="8">
-        <v>0</v>
-      </c>
+      <c r="L86" s="8"/>
       <c r="M86" s="11"/>
       <c r="N86" s="11"/>
       <c r="O86" s="10">
@@ -9249,9 +9211,7 @@
       <c r="K90" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L90" s="8">
-        <v>0</v>
-      </c>
+      <c r="L90" s="8"/>
       <c r="M90" s="11"/>
       <c r="N90" s="11"/>
       <c r="O90" s="10">
@@ -9852,9 +9812,7 @@
       <c r="K97" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L97" s="8">
-        <v>0</v>
-      </c>
+      <c r="L97" s="8"/>
       <c r="M97" s="9"/>
       <c r="N97" s="9"/>
       <c r="O97" s="10">
@@ -10026,9 +9984,7 @@
       <c r="K99" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L99" s="8">
-        <v>0</v>
-      </c>
+      <c r="L99" s="8"/>
       <c r="M99" s="9"/>
       <c r="N99" s="9"/>
       <c r="O99" s="10">
@@ -10113,9 +10069,7 @@
       <c r="K100" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L100" s="8">
-        <v>0</v>
-      </c>
+      <c r="L100" s="8"/>
       <c r="M100" s="9"/>
       <c r="N100" s="9"/>
       <c r="O100" s="10">
@@ -10372,9 +10326,7 @@
       <c r="K103" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L103" s="8">
-        <v>0</v>
-      </c>
+      <c r="L103" s="8"/>
       <c r="M103" s="9"/>
       <c r="N103" s="9"/>
       <c r="O103" s="10">
@@ -10459,9 +10411,7 @@
       <c r="K104" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L104" s="8">
-        <v>0</v>
-      </c>
+      <c r="L104" s="8"/>
       <c r="M104" s="9"/>
       <c r="N104" s="9"/>
       <c r="O104" s="10">

</xml_diff>